<commit_message>
Add boolean and date types to loading parameters from dataframe
Also small change to index the dataframe within the function
</commit_message>
<xml_diff>
--- a/tests/resources/ResourceFile_load-parameters.xlsx
+++ b/tests/resources/ResourceFile_load-parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/TLOmodel/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8D03BB-ED04-9144-A291-3E05C3BCE028}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A3E2EE-3C0B-654A-8C48-D855FF514AB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="-22580" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12620" yWindow="-14140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>parameter_name</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t xml:space="preserve">free_string </t>
+  </si>
+  <si>
+    <t>bool_true</t>
+  </si>
+  <si>
+    <t>bool_false</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -111,11 +120,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,11 +440,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -513,7 +521,32 @@
       </c>
       <c r="I7" s="2"/>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
+        <v>42036</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>